<commit_message>
Bringing everything up to date
</commit_message>
<xml_diff>
--- a/basinModel/BASE_top_elev - Copy.xlsx
+++ b/basinModel/BASE_top_elev - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f7dde64f327f866/UofA/2022-2023/Research/thesisCode_morales23/basinModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:40009_{E3B22705-0E5D-4112-995E-2F7644497AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39F76727-3EDE-43EB-811E-CB9240E96C4E}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:40009_{E3B22705-0E5D-4112-995E-2F7644497AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10734B5D-86C8-4C84-B43B-819530089454}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +455,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -646,7 +652,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -669,6 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -716,6 +723,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -935,6 +947,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1237,7 +1253,7 @@
   <dimension ref="A1:BK51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="CH37" sqref="CH37"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2208,7 +2224,7 @@
       <c r="AQ6">
         <v>95.3</v>
       </c>
-      <c r="AR6">
+      <c r="AR6" s="22">
         <v>95.2</v>
       </c>
       <c r="AS6">
@@ -2428,7 +2444,7 @@
       <c r="K8">
         <v>110</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="22">
         <v>109</v>
       </c>
       <c r="M8">
@@ -2817,7 +2833,7 @@
       <c r="AH10">
         <v>92.2</v>
       </c>
-      <c r="AI10">
+      <c r="AI10" s="20">
         <v>92.1</v>
       </c>
       <c r="AJ10">
@@ -2949,7 +2965,7 @@
       <c r="Z11">
         <v>92</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="22">
         <v>91.9</v>
       </c>
       <c r="AB11">
@@ -3058,7 +3074,7 @@
       <c r="I12">
         <v>108</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="22">
         <v>107</v>
       </c>
       <c r="K12">
@@ -3298,7 +3314,7 @@
       <c r="AK13">
         <v>88.9</v>
       </c>
-      <c r="AL13">
+      <c r="AL13" s="22">
         <v>88.8</v>
       </c>
       <c r="AM13">
@@ -3328,7 +3344,7 @@
       <c r="AU13">
         <v>87.9</v>
       </c>
-      <c r="AV13">
+      <c r="AV13" s="22">
         <v>87.8</v>
       </c>
       <c r="AW13">
@@ -3434,7 +3450,7 @@
       <c r="AC14">
         <v>88.7</v>
       </c>
-      <c r="AD14">
+      <c r="AD14" s="22">
         <v>88.6</v>
       </c>
       <c r="AE14">
@@ -3452,7 +3468,7 @@
       <c r="AI14">
         <v>88.1</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ14" s="22">
         <v>88</v>
       </c>
       <c r="AK14">
@@ -3895,7 +3911,7 @@
       <c r="Z17">
         <v>86</v>
       </c>
-      <c r="AA17">
+      <c r="AA17" s="22">
         <v>85.9</v>
       </c>
       <c r="AB17">
@@ -3940,7 +3956,7 @@
       <c r="AO17">
         <v>84.5</v>
       </c>
-      <c r="AP17">
+      <c r="AP17" s="22">
         <v>84.4</v>
       </c>
       <c r="AQ17">
@@ -4210,7 +4226,7 @@
       <c r="AA19">
         <v>83.9</v>
       </c>
-      <c r="AB19">
+      <c r="AB19" s="22">
         <v>83.8</v>
       </c>
       <c r="AC19">
@@ -4738,7 +4754,7 @@
       <c r="AU22">
         <v>78.900000000000006</v>
       </c>
-      <c r="AV22">
+      <c r="AV22" s="22">
         <v>78.8</v>
       </c>
       <c r="AW22">
@@ -5146,7 +5162,7 @@
       <c r="AA25">
         <v>77.900000000000006</v>
       </c>
-      <c r="AB25">
+      <c r="AB25" s="22">
         <v>77.8</v>
       </c>
       <c r="AC25">
@@ -5188,7 +5204,7 @@
       <c r="AO25">
         <v>76.5</v>
       </c>
-      <c r="AP25">
+      <c r="AP25" s="22">
         <v>76.400000000000006</v>
       </c>
       <c r="AQ25">
@@ -5326,7 +5342,7 @@
       <c r="AI26">
         <v>76.099999999999994</v>
       </c>
-      <c r="AJ26">
+      <c r="AJ26" s="22">
         <v>76</v>
       </c>
       <c r="AK26">
@@ -5617,7 +5633,7 @@
       <c r="AB28">
         <v>76.8</v>
       </c>
-      <c r="AC28">
+      <c r="AC28" s="22">
         <v>76.7</v>
       </c>
       <c r="AD28">
@@ -5821,7 +5837,7 @@
       <c r="AR29">
         <v>76.2</v>
       </c>
-      <c r="AS29">
+      <c r="AS29" s="22">
         <v>76.099999999999994</v>
       </c>
       <c r="AT29">
@@ -5953,7 +5969,7 @@
       <c r="AJ30">
         <v>78</v>
       </c>
-      <c r="AK30">
+      <c r="AK30" s="22">
         <v>77.900000000000006</v>
       </c>
       <c r="AL30">
@@ -6331,7 +6347,7 @@
       <c r="F33">
         <v>102</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="22">
         <v>101</v>
       </c>
       <c r="H33">
@@ -6922,7 +6938,7 @@
       <c r="AU36">
         <v>82.9</v>
       </c>
-      <c r="AV36">
+      <c r="AV36" s="22">
         <v>82.8</v>
       </c>
       <c r="AW36">
@@ -7021,7 +7037,7 @@
       <c r="AB37">
         <v>85.8</v>
       </c>
-      <c r="AC37">
+      <c r="AC37" s="22">
         <v>85.7</v>
       </c>
       <c r="AD37">
@@ -7204,7 +7220,7 @@
       <c r="AK38">
         <v>85.9</v>
       </c>
-      <c r="AL38">
+      <c r="AL38" s="22">
         <v>85.8</v>
       </c>
       <c r="AM38">
@@ -7630,7 +7646,7 @@
       <c r="W41">
         <v>93</v>
       </c>
-      <c r="X41">
+      <c r="X41" s="22">
         <v>92</v>
       </c>
       <c r="Y41">
@@ -7687,7 +7703,7 @@
       <c r="AP41">
         <v>88.4</v>
       </c>
-      <c r="AQ41">
+      <c r="AQ41" s="22">
         <v>88.3</v>
       </c>
       <c r="AR41">
@@ -7972,7 +7988,7 @@
       <c r="AG43">
         <v>91.3</v>
       </c>
-      <c r="AH43">
+      <c r="AH43" s="22">
         <v>91.2</v>
       </c>
       <c r="AI43">
@@ -9276,7 +9292,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:AY11 B23:AY30 B22:K22 AN22:AY22 B21:AY21 B20:S20 AG20:AQ20 AS20:AY20 B34:AY35 B33:AE33 AG33:AY33 B41:AY51 B40:K40 P40:AY40 B14:AY16 B13:N13 P13:AY13 M40:N40 B37:AY39 B36:T36 V36:AY36 V22:AD22 M22:T22 B12:T12 V12:AY12 B32:U32 AQ32:AY32 B18:AY19 B17:F17 AL17:AY17 AF22:AJ22 B31:T31 V31:AY31 H17:AJ17 W32:AO32 AL22 U20:AE20">
+  <conditionalFormatting sqref="B2:AY5 B23:AY24 B22:K22 AN22:AU22 B21:AY21 B20:S20 AG20:AQ20 AS20:AY20 B34:AY35 B33:F33 AG33:AY33 B42:AY42 B40:K40 P40:AY40 B15:AY16 B13:N13 P13:AK13 M40:N40 B37:AB37 B36:T36 V36:AU36 V22:AD22 M22:T22 B12:I12 V12:AY12 B32:U32 AQ32:AY32 B18:AY18 B17:F17 AL17:AO17 AF22:AJ22 B31:T31 V31:AY31 H17:Z17 W32:AO32 AL22 U20:AE20 B11:Z11 B10:AH10 AJ10:AY10 B7:AY7 B6:AQ6 AS6:AY6 AB17:AJ17 AM13:AU13 B39:AY39 B38:AK38 AM38:AY38 AD37:AY37 B30:AJ30 B28:AB28 AD28:AY28 B19:AA19 AC19:AY19 B27:AY27 B25:AA25 AC25:AO25 B26:AI26 AK26:AY26 AQ25:AY25 B29:AR29 AT29:AY29 AW36:AY36 B41:W41 AR41:AY41 B44:AY51 B43:AG43 AI43:AY43 Y41:AP41 K12:T12 B9:AY9 B8:K8 M8:AY8 AB11:AY11 B14:AC14 AE14:AI14 AK14:AY14 AW13:AY13 AQ17:AY17 AW22:AY22 AL30:AY30 H33:AE33">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>